<commit_message>
Modificaciones de vistas y funcionalidades
-Se modificó el fondo de la vista "tabla_editable" .
-Implementación de botones para eliminar etapas y aspectos.
-Se concluyo la opción de "Guardar Tabla" que ahora nos permite descargar la tabla en un documento excel.
</commit_message>
<xml_diff>
--- a/data/matriz_qfd.xlsx
+++ b/data/matriz_qfd.xlsx
@@ -441,17 +441,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>de</t>
+          <t>etapa 2</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>defr</t>
+          <t>etapa 3</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>cfytguh</t>
+          <t>dcfvg</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -463,45 +463,45 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sdef</t>
+          <t>sabor</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>def</t>
+          <t>precio</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>dtry</t>
+          <t>sdfg</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>